<commit_message>
update on 20210624 孤岛风云
</commit_message>
<xml_diff>
--- a/story/Activity Story 活动剧情/act11d0 Twilight of Wolumonde 沃伦姆德的薄暮 ウォルモンドの薄暮/level_act11d0_01_beg.xlsx
+++ b/story/Activity Story 活动剧情/act11d0 Twilight of Wolumonde 沃伦姆德的薄暮 ウォルモンドの薄暮/level_act11d0_01_beg.xlsx
@@ -1592,7 +1592,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">라이타니엔의 이동도시 월루몽드. 한때는 번화한 상업 도시였지만, 지금은 인적조차 드문 도시로 변해버렸다.
+    <t xml:space="preserve">라이타니아의 이동도시 월루몽드. 한때는 번화한 상업 도시였지만, 지금은 인적조차 드문 도시로 변해버렸다.
 </t>
   </si>
   <si>
@@ -1776,7 +1776,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[name="스즈란"]  여덟 번째 달이라는 뜻을 가진 월루몽드는, 주변의 일곱 도시와 함께 라이타니엔 서부에 번화한 상업지구를 형성했다……
+    <t xml:space="preserve">[name="스즈란"]  여덟 번째 달이라는 뜻을 가진 월루몽드는, 주변의 일곱 도시와 함께 라이타니아 서부에 번화한 상업지구를 형성했다……
 </t>
   </si>
   <si>
@@ -1824,7 +1824,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">[name="폴리닉"]  오리지늄 아츠의 보편화 덕분에 라이타니엔에는 다른 지역과는 다른 두 가지 특색이 생겼어. 하나는 음악 예술의 번영, 또 하나는 감염자에 대한 너그러운 태도지.
+    <t xml:space="preserve">[name="폴리닉"]  오리지늄 아츠의 보편화 덕분에 라이타니아에는 다른 지역과는 다른 두 가지 특색이 생겼어. 하나는 음악 예술의 번영, 또 하나는 감염자에 대한 너그러운 태도지.
 </t>
   </si>
   <si>

</xml_diff>